<commit_message>
support __default__ sheet in template file to format eval result xlsx file
</commit_message>
<xml_diff>
--- a/test/pipelines/eval_template.xlsx
+++ b/test/pipelines/eval_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Retriever" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Reader" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="__default__" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">multilabel_id</t>
   </si>
@@ -95,46 +95,13 @@
     <t xml:space="preserve">index</t>
   </si>
   <si>
-    <t xml:space="preserve">gold_answers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">answer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exact_match</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exact_match_context_scope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f1_context_scope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exact_match_document_id_scope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f1_document_id_scope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exact_match_document_id_and_context_scope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f1_document_id_and_context_scope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">offsets_in_document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gold_offsets_in_documents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gold_answers_exact_match</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gold_answers_f1</t>
+    <t xml:space="preserve">header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bar</t>
   </si>
 </sst>
 </file>
@@ -172,20 +139,33 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBF819E"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -193,13 +173,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -226,7 +199,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -239,16 +212,28 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -260,6 +245,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FFBF819E"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -270,8 +315,8 @@
   </sheetPr>
   <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z6" activeCellId="0" sqref="Z6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -280,7 +325,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="6" style="2" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -380,121 +425,36 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P28" activeCellId="0" sqref="P28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="7" style="2" width="8.53"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="4" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="5" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:N1048576">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFFF6D6D"/>
-        <color rgb="FFAFD095"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>